<commit_message>
Inserting Artist names and type, vendor
Initial sub-optimal insertion of artist info
</commit_message>
<xml_diff>
--- a/build_database/table validation 25 march.xlsx
+++ b/build_database/table validation 25 march.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\carbonarc\database_tool\build_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6B7796E3-19BF-44E8-A5D0-D84535799004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF9B9F3-A835-4A22-8761-38C32360F9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100"/>
+    <workbookView xWindow="41110" yWindow="1430" windowWidth="29250" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table validation" sheetId="1" r:id="rId1"/>
@@ -520,7 +520,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1088,27 +1088,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1126,16 +1106,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1448,11 +1418,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1812,10 +1782,10 @@
       <c r="J10">
         <v>24714</v>
       </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1879,10 +1849,10 @@
       <c r="J12">
         <v>24710</v>
       </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
         <v>0</v>
       </c>
     </row>
@@ -5461,7 +5431,7 @@
     <sortCondition ref="A2:A116"/>
   </sortState>
   <conditionalFormatting sqref="F2:H116">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Read in Multiple Map Table
Refactored so that the code can read in multiple map tables as well as as single thing table
</commit_message>
<xml_diff>
--- a/build_database/table validation 25 march.xlsx
+++ b/build_database/table validation 25 march.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\carbonarc\database_tool\build_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920AC895-90DF-4CAE-8442-6B99F423B4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FBAE6E-277B-40AF-9464-7AF63F549FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45840" yWindow="1910" windowWidth="29250" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1037,7 +1037,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1046,6 +1046,7 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1425,7 +1426,7 @@
   <dimension ref="A1:M116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1439,7 +1440,7 @@
     <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.26953125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.08984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="41.08984375" bestFit="1" customWidth="1"/>
@@ -1508,7 +1509,7 @@
       <c r="I2">
         <v>6</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="8">
         <v>10000</v>
       </c>
       <c r="K2">
@@ -1544,7 +1545,7 @@
       <c r="I3">
         <v>7</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="8">
         <v>10000</v>
       </c>
       <c r="K3">
@@ -1576,7 +1577,7 @@
       <c r="I4">
         <v>6</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="8">
         <v>45894</v>
       </c>
       <c r="K4">
@@ -1612,7 +1613,7 @@
       <c r="I5">
         <v>7</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="8">
         <v>35576</v>
       </c>
       <c r="K5">
@@ -1648,7 +1649,7 @@
       <c r="I6">
         <v>7</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="8">
         <v>1799</v>
       </c>
       <c r="M6" t="s">
@@ -1681,7 +1682,7 @@
       <c r="I7">
         <v>7</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="8">
         <v>27582</v>
       </c>
       <c r="K7">
@@ -1717,7 +1718,7 @@
       <c r="I8">
         <v>7</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="8">
         <v>47476</v>
       </c>
       <c r="K8">
@@ -1753,7 +1754,7 @@
       <c r="I9">
         <v>2</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="8">
         <v>63246</v>
       </c>
       <c r="M9" t="s">
@@ -1782,7 +1783,7 @@
       <c r="I10">
         <v>6</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="8">
         <v>24714</v>
       </c>
       <c r="K10" s="3">
@@ -1813,7 +1814,7 @@
       <c r="I11">
         <v>3</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="8">
         <v>0</v>
       </c>
       <c r="K11">
@@ -1849,7 +1850,7 @@
       <c r="I12">
         <v>7</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="8">
         <v>24710</v>
       </c>
       <c r="K12" s="3">
@@ -1885,7 +1886,7 @@
       <c r="I13">
         <v>7</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="8">
         <v>0</v>
       </c>
       <c r="K13">
@@ -1919,7 +1920,7 @@
       <c r="I14">
         <v>4</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="8">
         <v>0</v>
       </c>
       <c r="K14">
@@ -1955,7 +1956,7 @@
       <c r="I15">
         <v>4</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="8">
         <v>26432</v>
       </c>
       <c r="M15" t="s">
@@ -1988,7 +1989,7 @@
       <c r="I16">
         <v>7</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="8">
         <v>9654</v>
       </c>
       <c r="K16">
@@ -2024,7 +2025,7 @@
       <c r="I17">
         <v>7</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="8">
         <v>0</v>
       </c>
       <c r="K17">
@@ -2058,7 +2059,7 @@
       <c r="I18">
         <v>4</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="8">
         <v>0</v>
       </c>
       <c r="K18">
@@ -2094,7 +2095,7 @@
       <c r="I19">
         <v>7</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="8">
         <v>24339</v>
       </c>
       <c r="K19">
@@ -2130,7 +2131,7 @@
       <c r="I20">
         <v>7</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="8">
         <v>0</v>
       </c>
       <c r="K20">
@@ -2164,7 +2165,7 @@
       <c r="I21">
         <v>4</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="8">
         <v>0</v>
       </c>
       <c r="K21">
@@ -2200,7 +2201,7 @@
       <c r="I22">
         <v>7</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="8">
         <v>11968</v>
       </c>
       <c r="K22">
@@ -2236,7 +2237,7 @@
       <c r="I23">
         <v>7</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="8">
         <v>0</v>
       </c>
       <c r="K23">
@@ -2270,7 +2271,7 @@
       <c r="I24">
         <v>4</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="8">
         <v>0</v>
       </c>
       <c r="K24">
@@ -2284,7 +2285,7 @@
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C25" t="s">
@@ -2306,7 +2307,7 @@
       <c r="I25">
         <v>4</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="8">
         <v>4608</v>
       </c>
       <c r="K25">
@@ -2345,7 +2346,7 @@
       <c r="I26">
         <v>3</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="8">
         <v>94636</v>
       </c>
       <c r="M26" t="s">
@@ -2374,7 +2375,7 @@
       <c r="I27">
         <v>7</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="8">
         <v>74095</v>
       </c>
       <c r="K27">
@@ -2405,7 +2406,7 @@
       <c r="I28">
         <v>4</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="8">
         <v>0</v>
       </c>
       <c r="K28">
@@ -2437,7 +2438,7 @@
       <c r="I29">
         <v>6</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="8">
         <v>345</v>
       </c>
       <c r="K29">
@@ -2468,7 +2469,7 @@
       <c r="I30">
         <v>3</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="8">
         <v>0</v>
       </c>
       <c r="K30">
@@ -2500,7 +2501,7 @@
       <c r="I31">
         <v>11</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="8">
         <v>313</v>
       </c>
       <c r="K31">
@@ -2534,7 +2535,7 @@
       <c r="I32">
         <v>8</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="8">
         <v>0</v>
       </c>
       <c r="K32">
@@ -2569,7 +2570,7 @@
       <c r="I33">
         <v>8</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="8">
         <v>65508</v>
       </c>
       <c r="K33">
@@ -2600,7 +2601,7 @@
       <c r="I34">
         <v>4</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="8">
         <v>0</v>
       </c>
       <c r="K34">
@@ -2632,7 +2633,7 @@
       <c r="I35">
         <v>4</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="8">
         <v>9</v>
       </c>
       <c r="K35">
@@ -2667,7 +2668,7 @@
       <c r="I36">
         <v>6</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="8">
         <v>3</v>
       </c>
       <c r="K36">
@@ -2699,7 +2700,7 @@
       <c r="I37">
         <v>6</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="8">
         <v>7</v>
       </c>
       <c r="K37">
@@ -2735,7 +2736,7 @@
       <c r="I38">
         <v>7</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="8">
         <v>159</v>
       </c>
       <c r="K38">
@@ -2767,7 +2768,7 @@
       <c r="I39">
         <v>6</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="8">
         <v>825</v>
       </c>
       <c r="K39">
@@ -2799,7 +2800,7 @@
       <c r="I40">
         <v>6</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="8">
         <v>4</v>
       </c>
       <c r="K40">
@@ -2835,7 +2836,7 @@
       <c r="I41">
         <v>7</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="8">
         <v>6</v>
       </c>
       <c r="K41">
@@ -2867,7 +2868,7 @@
       <c r="I42">
         <v>6</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="8">
         <v>5</v>
       </c>
       <c r="K42">
@@ -2903,7 +2904,7 @@
       <c r="I43">
         <v>7</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="8">
         <v>85</v>
       </c>
       <c r="K43">
@@ -2935,7 +2936,7 @@
       <c r="I44">
         <v>6</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="8">
         <v>25</v>
       </c>
       <c r="K44">
@@ -2967,7 +2968,7 @@
       <c r="I45">
         <v>6</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="8">
         <v>2</v>
       </c>
       <c r="K45">
@@ -3006,7 +3007,7 @@
       <c r="I46">
         <v>7</v>
       </c>
-      <c r="J46">
+      <c r="J46" s="8">
         <v>11</v>
       </c>
       <c r="K46">
@@ -3038,7 +3039,7 @@
       <c r="I47">
         <v>6</v>
       </c>
-      <c r="J47">
+      <c r="J47" s="8">
         <v>4</v>
       </c>
       <c r="K47">
@@ -3074,7 +3075,7 @@
       <c r="I48">
         <v>7</v>
       </c>
-      <c r="J48">
+      <c r="J48" s="8">
         <v>9</v>
       </c>
       <c r="K48">
@@ -3106,7 +3107,7 @@
       <c r="I49">
         <v>6</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="8">
         <v>3</v>
       </c>
       <c r="K49">
@@ -3142,7 +3143,7 @@
       <c r="I50">
         <v>7</v>
       </c>
-      <c r="J50">
+      <c r="J50" s="8">
         <v>9</v>
       </c>
       <c r="K50">
@@ -3174,7 +3175,7 @@
       <c r="I51">
         <v>6</v>
       </c>
-      <c r="J51">
+      <c r="J51" s="8">
         <v>6</v>
       </c>
       <c r="K51">
@@ -3210,7 +3211,7 @@
       <c r="I52">
         <v>7</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="8">
         <v>14</v>
       </c>
       <c r="K52">
@@ -3242,7 +3243,7 @@
       <c r="I53">
         <v>8</v>
       </c>
-      <c r="J53">
+      <c r="J53" s="8">
         <v>74095</v>
       </c>
       <c r="K53">
@@ -3273,7 +3274,7 @@
       <c r="I54">
         <v>5</v>
       </c>
-      <c r="J54">
+      <c r="J54" s="8">
         <v>0</v>
       </c>
       <c r="K54">
@@ -3309,7 +3310,7 @@
       <c r="I55">
         <v>7</v>
       </c>
-      <c r="J55">
+      <c r="J55" s="8">
         <v>4017</v>
       </c>
       <c r="K55">
@@ -3345,7 +3346,7 @@
       <c r="I56">
         <v>7</v>
       </c>
-      <c r="J56">
+      <c r="J56" s="8">
         <v>0</v>
       </c>
       <c r="K56">
@@ -3379,7 +3380,7 @@
       <c r="I57">
         <v>4</v>
       </c>
-      <c r="J57">
+      <c r="J57" s="8">
         <v>0</v>
       </c>
       <c r="K57">
@@ -3415,7 +3416,7 @@
       <c r="I58">
         <v>7</v>
       </c>
-      <c r="J58">
+      <c r="J58" s="8">
         <v>1009</v>
       </c>
       <c r="K58">
@@ -3449,7 +3450,7 @@
       <c r="I59">
         <v>4</v>
       </c>
-      <c r="J59">
+      <c r="J59" s="8">
         <v>0</v>
       </c>
       <c r="K59">
@@ -3485,7 +3486,7 @@
       <c r="I60">
         <v>7</v>
       </c>
-      <c r="J60">
+      <c r="J60" s="8">
         <v>24031</v>
       </c>
       <c r="K60">
@@ -3521,7 +3522,7 @@
       <c r="I61">
         <v>7</v>
       </c>
-      <c r="J61">
+      <c r="J61" s="8">
         <v>0</v>
       </c>
       <c r="K61">
@@ -3555,7 +3556,7 @@
       <c r="I62">
         <v>4</v>
       </c>
-      <c r="J62">
+      <c r="J62" s="8">
         <v>0</v>
       </c>
       <c r="K62">
@@ -3591,7 +3592,7 @@
       <c r="I63">
         <v>7</v>
       </c>
-      <c r="J63">
+      <c r="J63" s="8">
         <v>1097</v>
       </c>
       <c r="K63">
@@ -3625,7 +3626,7 @@
       <c r="I64">
         <v>4</v>
       </c>
-      <c r="J64">
+      <c r="J64" s="8">
         <v>0</v>
       </c>
       <c r="K64">
@@ -3661,7 +3662,7 @@
       <c r="I65">
         <v>8</v>
       </c>
-      <c r="J65">
+      <c r="J65" s="8">
         <v>1578</v>
       </c>
       <c r="K65">
@@ -3697,7 +3698,7 @@
       <c r="I66">
         <v>7</v>
       </c>
-      <c r="J66">
+      <c r="J66" s="8">
         <v>0</v>
       </c>
       <c r="K66">
@@ -3731,7 +3732,7 @@
       <c r="I67">
         <v>5</v>
       </c>
-      <c r="J67">
+      <c r="J67" s="8">
         <v>0</v>
       </c>
       <c r="K67">
@@ -3767,7 +3768,7 @@
       <c r="I68">
         <v>7</v>
       </c>
-      <c r="J68">
+      <c r="J68" s="8">
         <v>1402</v>
       </c>
       <c r="K68">
@@ -3803,7 +3804,7 @@
       <c r="I69">
         <v>7</v>
       </c>
-      <c r="J69">
+      <c r="J69" s="8">
         <v>0</v>
       </c>
       <c r="K69">
@@ -3837,7 +3838,7 @@
       <c r="I70">
         <v>4</v>
       </c>
-      <c r="J70">
+      <c r="J70" s="8">
         <v>0</v>
       </c>
       <c r="K70">
@@ -3873,7 +3874,7 @@
       <c r="I71">
         <v>7</v>
       </c>
-      <c r="J71">
+      <c r="J71" s="8">
         <v>54301</v>
       </c>
       <c r="K71">
@@ -3909,7 +3910,7 @@
       <c r="I72">
         <v>7</v>
       </c>
-      <c r="J72">
+      <c r="J72" s="8">
         <v>0</v>
       </c>
       <c r="K72">
@@ -3943,7 +3944,7 @@
       <c r="I73">
         <v>4</v>
       </c>
-      <c r="J73">
+      <c r="J73" s="8">
         <v>0</v>
       </c>
       <c r="K73">
@@ -3979,7 +3980,7 @@
       <c r="I74">
         <v>7</v>
       </c>
-      <c r="J74">
+      <c r="J74" s="8">
         <v>11785</v>
       </c>
       <c r="K74">
@@ -4015,7 +4016,7 @@
       <c r="I75">
         <v>7</v>
       </c>
-      <c r="J75">
+      <c r="J75" s="8">
         <v>0</v>
       </c>
       <c r="K75">
@@ -4049,7 +4050,7 @@
       <c r="I76">
         <v>4</v>
       </c>
-      <c r="J76">
+      <c r="J76" s="8">
         <v>0</v>
       </c>
       <c r="K76">
@@ -4085,7 +4086,7 @@
       <c r="I77">
         <v>7</v>
       </c>
-      <c r="J77">
+      <c r="J77" s="8">
         <v>615</v>
       </c>
       <c r="K77">
@@ -4121,7 +4122,7 @@
       <c r="I78">
         <v>7</v>
       </c>
-      <c r="J78">
+      <c r="J78" s="8">
         <v>0</v>
       </c>
       <c r="K78">
@@ -4155,7 +4156,7 @@
       <c r="I79">
         <v>4</v>
       </c>
-      <c r="J79">
+      <c r="J79" s="8">
         <v>0</v>
       </c>
       <c r="K79">
@@ -4191,7 +4192,7 @@
       <c r="I80">
         <v>7</v>
       </c>
-      <c r="J80">
+      <c r="J80" s="8">
         <v>496</v>
       </c>
       <c r="K80">
@@ -4227,7 +4228,7 @@
       <c r="I81">
         <v>7</v>
       </c>
-      <c r="J81">
+      <c r="J81" s="8">
         <v>0</v>
       </c>
       <c r="K81">
@@ -4261,7 +4262,7 @@
       <c r="I82">
         <v>4</v>
       </c>
-      <c r="J82">
+      <c r="J82" s="8">
         <v>0</v>
       </c>
       <c r="K82">
@@ -4293,7 +4294,7 @@
       <c r="I83">
         <v>6</v>
       </c>
-      <c r="J83">
+      <c r="J83" s="8">
         <v>5</v>
       </c>
       <c r="K83">
@@ -4329,7 +4330,7 @@
       <c r="I84">
         <v>7</v>
       </c>
-      <c r="J84">
+      <c r="J84" s="8">
         <v>21</v>
       </c>
       <c r="K84">
@@ -4361,7 +4362,7 @@
       <c r="I85">
         <v>4</v>
       </c>
-      <c r="J85">
+      <c r="J85" s="8">
         <v>4</v>
       </c>
       <c r="K85">
@@ -4396,7 +4397,7 @@
       <c r="I86">
         <v>6</v>
       </c>
-      <c r="J86">
+      <c r="J86" s="8">
         <v>2</v>
       </c>
       <c r="K86">
@@ -4432,7 +4433,7 @@
       <c r="I87">
         <v>7</v>
       </c>
-      <c r="J87">
+      <c r="J87" s="8">
         <v>3</v>
       </c>
       <c r="K87">
@@ -4464,7 +4465,7 @@
       <c r="I88">
         <v>8</v>
       </c>
-      <c r="J88" s="2">
+      <c r="J88" s="8">
         <v>0</v>
       </c>
       <c r="K88">
@@ -4499,7 +4500,7 @@
       <c r="I89">
         <v>6</v>
       </c>
-      <c r="J89">
+      <c r="J89" s="8">
         <v>6</v>
       </c>
       <c r="K89">
@@ -4531,7 +4532,7 @@
       <c r="I90">
         <v>7</v>
       </c>
-      <c r="J90">
+      <c r="J90" s="8">
         <v>8</v>
       </c>
       <c r="K90">
@@ -4566,7 +4567,7 @@
       <c r="I91">
         <v>7</v>
       </c>
-      <c r="J91">
+      <c r="J91" s="8">
         <v>829</v>
       </c>
       <c r="K91">
@@ -4605,7 +4606,7 @@
       <c r="I92">
         <v>7</v>
       </c>
-      <c r="J92">
+      <c r="J92" s="8">
         <v>191</v>
       </c>
       <c r="M92" t="s">
@@ -4638,7 +4639,7 @@
       <c r="I93">
         <v>4</v>
       </c>
-      <c r="J93">
+      <c r="J93" s="8">
         <v>1052</v>
       </c>
       <c r="M93" t="s">
@@ -4667,7 +4668,7 @@
       <c r="I94">
         <v>7</v>
       </c>
-      <c r="J94">
+      <c r="J94" s="8">
         <v>829</v>
       </c>
       <c r="K94">
@@ -4702,7 +4703,7 @@
       <c r="I95">
         <v>7</v>
       </c>
-      <c r="J95">
+      <c r="J95" s="8">
         <v>51</v>
       </c>
       <c r="K95">
@@ -4734,7 +4735,7 @@
       <c r="I96">
         <v>6</v>
       </c>
-      <c r="J96">
+      <c r="J96" s="8">
         <v>753</v>
       </c>
       <c r="K96">
@@ -4766,7 +4767,7 @@
       <c r="I97">
         <v>8</v>
       </c>
-      <c r="J97">
+      <c r="J97" s="8">
         <v>0</v>
       </c>
       <c r="K97">
@@ -4801,7 +4802,7 @@
       <c r="I98">
         <v>6</v>
       </c>
-      <c r="J98">
+      <c r="J98" s="8">
         <v>0</v>
       </c>
       <c r="K98">
@@ -4836,7 +4837,7 @@
       <c r="I99">
         <v>6</v>
       </c>
-      <c r="J99">
+      <c r="J99" s="8">
         <v>0</v>
       </c>
       <c r="K99">
@@ -4871,7 +4872,7 @@
       <c r="I100">
         <v>6</v>
       </c>
-      <c r="J100">
+      <c r="J100" s="8">
         <v>44738</v>
       </c>
       <c r="K100">
@@ -4902,7 +4903,7 @@
       <c r="I101">
         <v>5</v>
       </c>
-      <c r="J101">
+      <c r="J101" s="8">
         <v>0</v>
       </c>
       <c r="K101">
@@ -4938,7 +4939,7 @@
       <c r="I102">
         <v>6</v>
       </c>
-      <c r="J102">
+      <c r="J102" s="8">
         <v>26610</v>
       </c>
       <c r="K102">
@@ -4974,7 +4975,7 @@
       <c r="I103">
         <v>7</v>
       </c>
-      <c r="J103">
+      <c r="J103" s="8">
         <v>0</v>
       </c>
       <c r="K103">
@@ -5008,7 +5009,7 @@
       <c r="I104">
         <v>4</v>
       </c>
-      <c r="J104">
+      <c r="J104" s="8">
         <v>0</v>
       </c>
       <c r="K104">
@@ -5044,7 +5045,7 @@
       <c r="I105">
         <v>6</v>
       </c>
-      <c r="J105">
+      <c r="J105" s="8">
         <v>18128</v>
       </c>
       <c r="K105">
@@ -5076,7 +5077,7 @@
       <c r="I106">
         <v>14</v>
       </c>
-      <c r="J106">
+      <c r="J106" s="8">
         <v>10352</v>
       </c>
       <c r="K106">
@@ -5107,7 +5108,7 @@
       <c r="I107">
         <v>11</v>
       </c>
-      <c r="J107">
+      <c r="J107" s="8">
         <v>0</v>
       </c>
       <c r="K107">
@@ -5138,7 +5139,7 @@
       <c r="I108">
         <v>19</v>
       </c>
-      <c r="J108">
+      <c r="J108" s="8">
         <v>0</v>
       </c>
       <c r="K108">
@@ -5174,7 +5175,7 @@
       <c r="I109">
         <v>7</v>
       </c>
-      <c r="J109">
+      <c r="J109" s="8">
         <v>10224</v>
       </c>
       <c r="K109">
@@ -5208,7 +5209,7 @@
       <c r="I110">
         <v>4</v>
       </c>
-      <c r="J110">
+      <c r="J110" s="8">
         <v>0</v>
       </c>
       <c r="K110">
@@ -5244,7 +5245,7 @@
       <c r="I111">
         <v>6</v>
       </c>
-      <c r="J111">
+      <c r="J111" s="8">
         <v>894</v>
       </c>
       <c r="K111" s="2">
@@ -5281,7 +5282,7 @@
       <c r="I112">
         <v>4</v>
       </c>
-      <c r="J112">
+      <c r="J112" s="8">
         <v>0</v>
       </c>
       <c r="K112">
@@ -5317,7 +5318,7 @@
       <c r="I113">
         <v>6</v>
       </c>
-      <c r="J113">
+      <c r="J113" s="8">
         <v>991</v>
       </c>
       <c r="K113">
@@ -5351,7 +5352,7 @@
       <c r="I114">
         <v>4</v>
       </c>
-      <c r="J114">
+      <c r="J114" s="8">
         <v>0</v>
       </c>
       <c r="K114">
@@ -5383,7 +5384,7 @@
       <c r="I115">
         <v>6</v>
       </c>
-      <c r="J115">
+      <c r="J115" s="8">
         <v>5</v>
       </c>
       <c r="K115">
@@ -5419,7 +5420,7 @@
       <c r="I116">
         <v>7</v>
       </c>
-      <c r="J116">
+      <c r="J116" s="8">
         <v>39</v>
       </c>
       <c r="K116">

</xml_diff>

<commit_message>
Added in most tables and vendors
Added in extra data columns to all tables. Need to fill them in next.
</commit_message>
<xml_diff>
--- a/build_database/table validation 25 march.xlsx
+++ b/build_database/table validation 25 march.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\carbonarc\database_tool\build_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98149746-78AB-40F2-803F-FBFFB430A52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9208E7D6-C9E7-4F0A-9B99-9178F90F9272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42050" yWindow="1780" windowWidth="33520" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52510" yWindow="750" windowWidth="22620" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table validation" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="169">
   <si>
     <t>table_name</t>
   </si>
@@ -534,6 +534,15 @@
   </si>
   <si>
     <t>half log, no primary key</t>
+  </si>
+  <si>
+    <t>extra unknow column (tag?)</t>
+  </si>
+  <si>
+    <t>Not sure about the name ferret_retailer</t>
+  </si>
+  <si>
+    <t>2 extra columns, both are all null values</t>
   </si>
 </sst>
 </file>
@@ -676,7 +685,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -892,6 +901,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1053,7 +1068,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1063,6 +1078,7 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1442,8 +1458,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:M116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33:E33"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1508,24 +1524,24 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="3">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="9">
         <v>6</v>
       </c>
       <c r="J2" s="8">
@@ -1542,26 +1558,26 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3">
+      <c r="F3" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
         <v>7</v>
       </c>
       <c r="J3" s="8">
@@ -1578,24 +1594,24 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
         <v>6</v>
       </c>
       <c r="J4" s="8">
@@ -1612,26 +1628,26 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5">
+      <c r="F5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
         <v>7</v>
       </c>
       <c r="J5" s="8">
@@ -1660,11 +1676,11 @@
       <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1" t="b">
+      <c r="F6" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6" t="b">
         <v>0</v>
       </c>
       <c r="I6">
@@ -1681,26 +1697,26 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7">
+      <c r="F7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
         <v>7</v>
       </c>
       <c r="J7" s="8">
@@ -1717,26 +1733,26 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I8">
+      <c r="F8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
         <v>7</v>
       </c>
       <c r="J8" s="8">
@@ -1765,11 +1781,11 @@
       <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1" t="b">
+      <c r="F9" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6" t="b">
         <v>0</v>
       </c>
       <c r="I9">
@@ -1786,24 +1802,24 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="3">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="9">
         <v>6</v>
       </c>
       <c r="J10" s="8">
@@ -1851,26 +1867,26 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="3">
+      <c r="F12" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="9">
         <v>7</v>
       </c>
       <c r="J12" s="8">
@@ -1969,11 +1985,11 @@
       <c r="E15" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1" t="b">
+      <c r="F15" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6" t="b">
         <v>0</v>
       </c>
       <c r="I15">
@@ -1990,26 +2006,26 @@
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" s="3">
+      <c r="F16" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9">
         <v>7</v>
       </c>
       <c r="J16" s="8">
@@ -2096,26 +2112,26 @@
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="F19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="3">
+      <c r="F19" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="9">
         <v>7</v>
       </c>
       <c r="J19" s="8">
@@ -2202,26 +2218,26 @@
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" s="3">
+      <c r="F22" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="9">
         <v>7</v>
       </c>
       <c r="J22" s="8">
@@ -2308,26 +2324,26 @@
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" s="3">
+      <c r="F25" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="9">
         <v>4</v>
       </c>
       <c r="J25" s="8">
@@ -2359,11 +2375,11 @@
       <c r="E26" t="s">
         <v>51</v>
       </c>
-      <c r="F26" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1" t="b">
+      <c r="F26" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6" t="b">
         <v>0</v>
       </c>
       <c r="I26">
@@ -2380,24 +2396,24 @@
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G27" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H27" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I27">
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="4">
         <v>7</v>
       </c>
       <c r="J27" s="8">
@@ -2445,24 +2461,24 @@
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H29" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I29">
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" s="9">
         <v>6</v>
       </c>
       <c r="J29" s="8">
@@ -2510,19 +2526,19 @@
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F31" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G31" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H31" s="1" t="b">
+      <c r="F31" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I31">
@@ -2579,24 +2595,24 @@
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G33" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I33">
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G33" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I33" s="4">
         <v>8</v>
       </c>
       <c r="J33" s="8">
@@ -2607,6 +2623,9 @@
       </c>
       <c r="L33">
         <v>0</v>
+      </c>
+      <c r="M33" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
@@ -2644,19 +2663,19 @@
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C35" t="s">
         <v>59</v>
       </c>
-      <c r="F35" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G35" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" s="1" t="b">
+      <c r="F35" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G35" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" s="6" t="b">
         <v>0</v>
       </c>
       <c r="I35">
@@ -2679,22 +2698,24 @@
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F36" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G36" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I36">
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I36" s="9">
         <v>6</v>
       </c>
       <c r="J36" s="8">
@@ -2711,22 +2732,24 @@
       <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F37" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G37" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I37">
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G37" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I37" s="9">
         <v>6</v>
       </c>
       <c r="J37" s="8">
@@ -2743,26 +2766,26 @@
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I38">
+      <c r="F38" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I38" s="9">
         <v>7</v>
       </c>
       <c r="J38" s="8">
@@ -2779,22 +2802,24 @@
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F39" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G39" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I39">
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G39" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I39" s="9">
         <v>6</v>
       </c>
       <c r="J39" s="8">
@@ -2811,22 +2836,24 @@
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F40" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G40" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I40">
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G40" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="9">
         <v>6</v>
       </c>
       <c r="J40" s="8">
@@ -2843,26 +2870,26 @@
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F41" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I41">
+      <c r="F41" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I41" s="9">
         <v>7</v>
       </c>
       <c r="J41" s="8">
@@ -2879,22 +2906,24 @@
       <c r="A42">
         <v>40</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F42" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G42" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H42" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I42">
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G42" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" s="9">
         <v>6</v>
       </c>
       <c r="J42" s="8">
@@ -2911,26 +2940,26 @@
       <c r="A43">
         <v>41</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F43" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I43">
+      <c r="F43" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" s="9">
         <v>7</v>
       </c>
       <c r="J43" s="8">
@@ -2947,22 +2976,24 @@
       <c r="A44">
         <v>42</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="F44" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G44" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H44" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I44">
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G44" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" s="9">
         <v>6</v>
       </c>
       <c r="J44" s="8">
@@ -2979,19 +3010,19 @@
       <c r="A45">
         <v>43</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F45" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G45" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H45" s="1" t="b">
+      <c r="F45" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G45" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H45" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I45">
@@ -3014,10 +3045,10 @@
       <c r="A46">
         <v>44</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D46" t="s">
@@ -3026,11 +3057,11 @@
       <c r="E46" t="s">
         <v>63</v>
       </c>
-      <c r="F46" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1" t="b">
+      <c r="F46" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I46">
@@ -3050,22 +3081,24 @@
       <c r="A47">
         <v>45</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F47" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G47" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H47" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I47">
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G47" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" s="9">
         <v>6</v>
       </c>
       <c r="J47" s="8">
@@ -3082,26 +3115,26 @@
       <c r="A48">
         <v>46</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F48" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I48">
+      <c r="F48" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" s="9">
         <v>7</v>
       </c>
       <c r="J48" s="8">
@@ -3114,26 +3147,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>47</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F49" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G49" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H49" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I49">
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G49" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" s="9">
         <v>6</v>
       </c>
       <c r="J49" s="8">
@@ -3146,30 +3181,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>48</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F50" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I50">
+      <c r="F50" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" s="9">
         <v>7</v>
       </c>
       <c r="J50" s="8">
@@ -3182,26 +3217,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>49</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F51" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G51" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H51" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I51">
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G51" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I51" s="9">
         <v>6</v>
       </c>
       <c r="J51" s="8">
@@ -3214,30 +3251,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>50</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F52" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I52">
+      <c r="F52" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" s="9">
         <v>7</v>
       </c>
       <c r="J52" s="8">
@@ -3250,26 +3287,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>51</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F53" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G53" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H53" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I53">
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G53" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I53" s="4">
         <v>8</v>
       </c>
       <c r="J53" s="8">
@@ -3282,7 +3321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3313,30 +3352,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>53</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F55" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I55">
+      <c r="F55" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I55" s="9">
         <v>7</v>
       </c>
       <c r="J55" s="8">
@@ -3349,7 +3388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>54</v>
       </c>
@@ -3385,7 +3424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>55</v>
       </c>
@@ -3419,30 +3458,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>56</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F58" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I58">
+      <c r="F58" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I58" s="9">
         <v>7</v>
       </c>
       <c r="J58" s="8">
@@ -3455,7 +3494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>57</v>
       </c>
@@ -3489,30 +3528,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>58</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F60" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I60">
+      <c r="F60" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I60" s="9">
         <v>7</v>
       </c>
       <c r="J60" s="8">
@@ -3525,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3561,7 +3600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>60</v>
       </c>
@@ -3595,30 +3634,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>61</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F63" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I63">
+      <c r="F63" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I63" s="9">
         <v>7</v>
       </c>
       <c r="J63" s="8">
@@ -3630,8 +3669,11 @@
       <c r="L63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M63" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3665,30 +3707,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>63</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F65" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I65">
+      <c r="F65" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I65" s="4">
         <v>8</v>
       </c>
       <c r="J65" s="8">
@@ -3700,8 +3742,11 @@
       <c r="L65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+      <c r="M65" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3737,7 +3782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3771,30 +3816,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>66</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F68" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I68">
+      <c r="F68" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I68" s="9">
         <v>7</v>
       </c>
       <c r="J68" s="8">
@@ -3807,7 +3852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3843,7 +3888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3877,30 +3922,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>69</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F71" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I71">
+      <c r="F71" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I71" s="9">
         <v>7</v>
       </c>
       <c r="J71" s="8">
@@ -3913,7 +3958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3949,7 +3994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3983,30 +4028,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>72</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C74" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F74" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I74">
+      <c r="F74" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I74" s="9">
         <v>7</v>
       </c>
       <c r="J74" s="8">
@@ -4019,7 +4064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>73</v>
       </c>
@@ -4055,7 +4100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>74</v>
       </c>
@@ -4089,30 +4134,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>75</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F77" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I77">
+      <c r="F77" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I77" s="9">
         <v>7</v>
       </c>
       <c r="J77" s="8">
@@ -4125,7 +4170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>76</v>
       </c>
@@ -4161,7 +4206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>77</v>
       </c>
@@ -4195,30 +4240,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>78</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F80" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I80">
+      <c r="F80" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I80" s="9">
         <v>7</v>
       </c>
       <c r="J80" s="8">
@@ -4305,22 +4350,24 @@
       <c r="A83">
         <v>81</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="F83" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G83" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H83" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I83">
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G83" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H83" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I83" s="9">
         <v>6</v>
       </c>
       <c r="J83" s="8">
@@ -4337,26 +4384,26 @@
       <c r="A84">
         <v>82</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F84" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I84">
+      <c r="F84" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I84" s="9">
         <v>7</v>
       </c>
       <c r="J84" s="8">
@@ -4373,22 +4420,24 @@
       <c r="A85">
         <v>83</v>
       </c>
-      <c r="B85" s="3" t="s">
+      <c r="B85" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F85" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G85" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H85" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I85">
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G85" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H85" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I85" s="9">
         <v>4</v>
       </c>
       <c r="J85" s="8">
@@ -4408,22 +4457,24 @@
       <c r="A86">
         <v>84</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="F86" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G86" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H86" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I86">
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G86" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H86" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I86" s="9">
         <v>6</v>
       </c>
       <c r="J86" s="8">
@@ -4440,26 +4491,26 @@
       <c r="A87">
         <v>85</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D87" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F87" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I87">
+      <c r="F87" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I87" s="9">
         <v>7</v>
       </c>
       <c r="J87" s="8">
@@ -4476,19 +4527,19 @@
       <c r="A88">
         <v>86</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="4" t="s">
         <v>119</v>
       </c>
       <c r="C88" t="s">
         <v>119</v>
       </c>
-      <c r="F88" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G88" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H88" s="1" t="b">
+      <c r="F88" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G88" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H88" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I88">
@@ -4511,22 +4562,24 @@
       <c r="A89">
         <v>87</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="F89" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G89" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H89" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I89">
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G89" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H89" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I89" s="9">
         <v>6</v>
       </c>
       <c r="J89" s="8">
@@ -4543,19 +4596,19 @@
       <c r="A90">
         <v>88</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="4" t="s">
         <v>121</v>
       </c>
       <c r="C90" t="s">
         <v>121</v>
       </c>
-      <c r="F90" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G90" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H90" s="1" t="b">
+      <c r="F90" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G90" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H90" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I90">
@@ -4578,19 +4631,19 @@
       <c r="A91">
         <v>89</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="4" t="s">
         <v>122</v>
       </c>
       <c r="C91" t="s">
         <v>122</v>
       </c>
-      <c r="F91" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G91" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H91" s="1" t="b">
+      <c r="F91" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G91" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H91" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I91">
@@ -4613,7 +4666,7 @@
       <c r="A92">
         <v>90</v>
       </c>
-      <c r="B92" s="3" t="s">
+      <c r="B92" s="4" t="s">
         <v>123</v>
       </c>
       <c r="C92" t="s">
@@ -4625,11 +4678,11 @@
       <c r="E92" t="s">
         <v>124</v>
       </c>
-      <c r="F92" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1" t="b">
+      <c r="F92" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I92">
@@ -4646,7 +4699,7 @@
       <c r="A93">
         <v>91</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="B93" s="4" t="s">
         <v>125</v>
       </c>
       <c r="C93" t="s">
@@ -4658,11 +4711,11 @@
       <c r="E93" t="s">
         <v>49</v>
       </c>
-      <c r="F93" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1" t="b">
+      <c r="F93" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6" t="b">
         <v>0</v>
       </c>
       <c r="I93">
@@ -4679,19 +4732,19 @@
       <c r="A94">
         <v>92</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C94" t="s">
         <v>126</v>
       </c>
-      <c r="F94" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G94" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H94" s="1" t="b">
+      <c r="F94" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G94" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H94" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I94">
@@ -4714,22 +4767,24 @@
       <c r="A95">
         <v>93</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F95" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G95" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H95" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I95">
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G95" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H95" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I95" s="4">
         <v>7</v>
       </c>
       <c r="J95" s="8">
@@ -4746,22 +4801,24 @@
       <c r="A96">
         <v>94</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F96" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G96" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H96" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I96">
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G96" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H96" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I96" s="9">
         <v>6</v>
       </c>
       <c r="J96" s="8">
@@ -4784,13 +4841,13 @@
       <c r="C97" t="s">
         <v>129</v>
       </c>
-      <c r="F97" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G97" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H97" s="1" t="b">
+      <c r="F97" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G97" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="H97" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I97">
@@ -4819,13 +4876,13 @@
       <c r="C98" t="s">
         <v>130</v>
       </c>
-      <c r="F98" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G98" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H98" s="1" t="b">
+      <c r="F98" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G98" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H98" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I98">
@@ -4854,13 +4911,13 @@
       <c r="C99" t="s">
         <v>131</v>
       </c>
-      <c r="F99" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G99" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H99" s="1" t="b">
+      <c r="F99" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G99" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H99" s="6" t="b">
         <v>1</v>
       </c>
       <c r="I99">
@@ -4883,22 +4940,24 @@
       <c r="A100">
         <v>98</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F100" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G100" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H100" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I100">
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G100" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H100" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I100" s="9">
         <v>6</v>
       </c>
       <c r="J100" s="8">
@@ -4946,26 +5005,26 @@
       <c r="A102">
         <v>100</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D102" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F102" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I102">
+      <c r="F102" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I102" s="9">
         <v>6</v>
       </c>
       <c r="J102" s="8">
@@ -5052,26 +5111,26 @@
       <c r="A105">
         <v>103</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D105" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E105" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="F105" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G105" s="1"/>
-      <c r="H105" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I105">
+      <c r="F105" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I105" s="9">
         <v>6</v>
       </c>
       <c r="J105" s="8">
@@ -5088,22 +5147,24 @@
       <c r="A106">
         <v>104</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F106" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G106" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H106" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I106">
+      <c r="D106" s="9"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G106" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H106" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I106" s="4">
         <v>14</v>
       </c>
       <c r="J106" s="8">
@@ -5182,26 +5243,26 @@
       <c r="A109">
         <v>107</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D109" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E109" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F109" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G109" s="1"/>
-      <c r="H109" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I109">
+      <c r="F109" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I109" s="9">
         <v>7</v>
       </c>
       <c r="J109" s="8">
@@ -5264,11 +5325,11 @@
       <c r="E111" t="s">
         <v>124</v>
       </c>
-      <c r="F111" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G111" s="1"/>
-      <c r="H111" s="1" t="b">
+      <c r="F111" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6" t="b">
         <v>0</v>
       </c>
       <c r="I111">
@@ -5325,26 +5386,26 @@
       <c r="A113">
         <v>111</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D113" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E113" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F113" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G113" s="1"/>
-      <c r="H113" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I113">
+      <c r="F113" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I113" s="9">
         <v>6</v>
       </c>
       <c r="J113" s="8">
@@ -5395,22 +5456,24 @@
       <c r="A115">
         <v>113</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C115" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F115" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G115" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H115" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I115">
+      <c r="D115" s="9"/>
+      <c r="E115" s="9"/>
+      <c r="F115" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G115" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H115" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I115" s="9">
         <v>6</v>
       </c>
       <c r="J115" s="8">
@@ -5427,26 +5490,26 @@
       <c r="A116">
         <v>114</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C116" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F116" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G116" s="1"/>
-      <c r="H116" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I116">
+      <c r="F116" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I116" s="9">
         <v>7</v>
       </c>
       <c r="J116" s="8">

</xml_diff>